<commit_message>
Implementing correct ph,stroma/ph,lumen. Vr implemented.
Implementing correct ph,stroma/ph,lumen. Vr implemented.
</commit_message>
<xml_diff>
--- a/FRR_with_ATP_synthase_Model_Kramer/LaiskReactions1.xlsx
+++ b/FRR_with_ATP_synthase_Model_Kramer/LaiskReactions1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/Laisk-PSII/FRR_with_ATP_synthase_Model_Kramer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FBE10727-9731-B343-BF12-1FF1CD1FB330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2B41C6AC-2D7A-D448-BE2A-542683996646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11280" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11280" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1381,8 +1381,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="130" workbookViewId="0">
-      <selection activeCell="A263" sqref="A263"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="130" workbookViewId="0">
+      <selection activeCell="B271" sqref="B271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3779,15 +3779,15 @@
         <v>298</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>299</v>
       </c>
-      <c r="B271" s="2" t="s">
-        <v>287</v>
+      <c r="B271" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>